<commit_message>
started uml work on burndown chart
</commit_message>
<xml_diff>
--- a/burndown.xlsx
+++ b/burndown.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t xml:space="preserve">AGILE SPRINT BACKLOG TEMPLATE WITH BURNDOWN CHART</t>
   </si>
@@ -54,13 +54,22 @@
     <t xml:space="preserve">User Story #1</t>
   </si>
   <si>
-    <t xml:space="preserve">Task </t>
+    <t xml:space="preserve">Create UML Diagram</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In Progress</t>
   </si>
   <si>
     <t>Task</t>
   </si>
   <si>
     <t xml:space="preserve">User Story #2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task </t>
   </si>
   <si>
     <t xml:space="preserve">User Story #3</t>
@@ -1090,7 +1099,7 @@
       </c>
       <c r="C3" s="7">
         <f>SUM(C4:C7)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
@@ -1123,11 +1132,21 @@
       <c r="B4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
+      <c r="C4" s="9">
+        <v>1</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="10">
+        <v>3</v>
+      </c>
+      <c r="G4" s="10">
+        <v>1</v>
+      </c>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
       <c r="J4" s="9"/>
@@ -1152,9 +1171,7 @@
     </row>
     <row r="5" ht="24.75" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="B5" s="9"/>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
@@ -1185,7 +1202,7 @@
     <row r="6" ht="24.75" customHeight="1">
       <c r="A6" s="1"/>
       <c r="B6" s="9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -1217,7 +1234,7 @@
     <row r="7" ht="24.75" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
@@ -1249,7 +1266,7 @@
     <row r="8" ht="24.75" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="8"/>
@@ -1281,7 +1298,7 @@
     <row r="9" ht="24.75" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="9" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
@@ -1313,7 +1330,7 @@
     <row r="10" ht="24.75" customHeight="1">
       <c r="A10" s="1"/>
       <c r="B10" s="9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
@@ -1345,7 +1362,7 @@
     <row r="11" ht="24.75" customHeight="1">
       <c r="A11" s="1"/>
       <c r="B11" s="9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
@@ -1377,7 +1394,7 @@
     <row r="12" ht="24.75" customHeight="1">
       <c r="A12" s="1"/>
       <c r="B12" s="9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
@@ -1409,7 +1426,7 @@
     <row r="13" ht="24.75" customHeight="1">
       <c r="A13" s="1"/>
       <c r="B13" s="7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="8"/>
@@ -1441,7 +1458,7 @@
     <row r="14" ht="24.75" customHeight="1">
       <c r="A14" s="1"/>
       <c r="B14" s="9" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
@@ -1473,7 +1490,7 @@
     <row r="15" ht="24.75" customHeight="1">
       <c r="A15" s="1"/>
       <c r="B15" s="9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
@@ -1505,7 +1522,7 @@
     <row r="16" ht="24.75" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
@@ -1537,7 +1554,7 @@
     <row r="17" ht="24.75" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
@@ -1569,7 +1586,7 @@
     <row r="18" ht="24.75" customHeight="1">
       <c r="A18" s="1"/>
       <c r="B18" s="7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="8"/>
@@ -1601,7 +1618,7 @@
     <row r="19" ht="24.75" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="9" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
@@ -1633,7 +1650,7 @@
     <row r="20" ht="24.75" customHeight="1">
       <c r="A20" s="1"/>
       <c r="B20" s="9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
@@ -1665,7 +1682,7 @@
     <row r="21" ht="24.75" customHeight="1">
       <c r="A21" s="1"/>
       <c r="B21" s="9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
@@ -1697,7 +1714,7 @@
     <row r="22" ht="24.75" customHeight="1">
       <c r="A22" s="1"/>
       <c r="B22" s="9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
@@ -1729,7 +1746,7 @@
     <row r="23" ht="24.75" customHeight="1">
       <c r="A23" s="1"/>
       <c r="B23" s="7" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="8"/>
@@ -1761,7 +1778,7 @@
     <row r="24" ht="24.75" customHeight="1">
       <c r="A24" s="1"/>
       <c r="B24" s="9" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
@@ -1793,7 +1810,7 @@
     <row r="25" ht="24.75" customHeight="1">
       <c r="A25" s="1"/>
       <c r="B25" s="9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
@@ -1825,7 +1842,7 @@
     <row r="26" ht="24.75" customHeight="1">
       <c r="A26" s="1"/>
       <c r="B26" s="9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
@@ -1857,7 +1874,7 @@
     <row r="27" ht="24.75" customHeight="1">
       <c r="A27" s="1"/>
       <c r="B27" s="9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
@@ -1889,18 +1906,18 @@
     <row r="28" ht="34.5" customHeight="1">
       <c r="A28" s="1"/>
       <c r="B28" s="11" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C28" s="11"/>
       <c r="D28" s="11"/>
       <c r="E28" s="11"/>
       <c r="F28" s="11">
         <f>SUM(F3:F27)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G28" s="12">
         <f>SUM(G4:G27)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H28" s="11">
         <f t="shared" ref="H28:L28" si="0">SUM(H3:H27)</f>

</xml_diff>

<commit_message>
added Day 2 to burndown
</commit_message>
<xml_diff>
--- a/burndown.xlsx
+++ b/burndown.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
   <si>
     <t xml:space="preserve">AGILE SPRINT BACKLOG TEMPLATE WITH BURNDOWN CHART</t>
   </si>
@@ -373,7 +373,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -555,11 +555,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="61842063"/>
-        <c:axId val="65697678"/>
+        <c:axId val="32761173"/>
+        <c:axId val="89991301"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="61842063"/>
+        <c:axId val="32761173"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -592,7 +592,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65697678"/>
+        <c:crossAx val="89991301"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -600,7 +600,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="65697678"/>
+        <c:axId val="89991301"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -643,7 +643,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61842063"/>
+        <c:crossAx val="32761173"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -717,7 +717,7 @@
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
+      <selection pane="bottomLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.22265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -899,7 +899,9 @@
     </row>
     <row r="5" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
-      <c r="B5" s="7"/>
+      <c r="B5" s="7" t="s">
+        <v>16</v>
+      </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>

</xml_diff>